<commit_message>
updated files to add motorbikes freight data
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLRaPTC/Annual Vehicle Licensing Registration and Property Tax Costs.xlsx
+++ b/InputData/trans/AVLRaPTC/Annual Vehicle Licensing Registration and Property Tax Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\AVLRaPTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\trans\AVLRaPTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D32A06-ED03-485E-BDB4-2BF12EEC6254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F482D24-75E5-4543-869B-25E5DC2E7F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33735" yWindow="675" windowWidth="21600" windowHeight="22305" xr2:uid="{AF599D04-C13D-45D7-BEF0-770B4B16FC27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{AF599D04-C13D-45D7-BEF0-770B4B16FC27}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC3CD7F-A224-4C3A-9A5E-D38F07B136AE}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -732,7 +732,9 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -818,8 +820,9 @@
         <f>$B$2*About!$A$30</f>
         <v>338.09699999999998</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" s="8">
+        <f>C3</f>
+        <v>1352.3879999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>